<commit_message>
MethodNotAllowedHttpException redirect to 404
</commit_message>
<xml_diff>
--- a/me-docs/30.Gioi-han-vung-truy-cap.xlsx
+++ b/me-docs/30.Gioi-han-vung-truy-cap.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\proj_news\me-docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA525B7-79DA-4BA2-B30C-6539439E9B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1611828-70E1-49D1-B802-9A4421FB8D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login template" sheetId="1" r:id="rId1"/>
     <sheet name="validate" sheetId="2" r:id="rId2"/>
     <sheet name="login" sheetId="3" r:id="rId3"/>
+    <sheet name="MethodNotAllowedHttpException" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>proj\routes\web.php</t>
   </si>
@@ -69,6 +70,21 @@
   </si>
   <si>
     <t>resources\lang\en\notify.php</t>
+  </si>
+  <si>
+    <t>Access to post method</t>
+  </si>
+  <si>
+    <t>routes\web.php</t>
+  </si>
+  <si>
+    <t>MethodNotAllowedHttpException redirect to 404</t>
+  </si>
+  <si>
+    <t>app\Exceptions\Handler.php</t>
+  </si>
+  <si>
+    <t>Access http://proj_news.xyz/blog/postLogin</t>
   </si>
 </sst>
 </file>
@@ -1139,6 +1155,275 @@
         <a:xfrm>
           <a:off x="609600" y="5524500"/>
           <a:ext cx="8495238" cy="3133333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>8152</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>75881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E026659B-7DCB-3EB2-FB61-06470951207F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="762000"/>
+          <a:ext cx="10980952" cy="2552381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>131537</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17A233FD-B3F7-379A-3C3D-244639ABD3EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="3238500"/>
+          <a:ext cx="11401425" cy="5275037"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>151390</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>142643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CF1FA88-3AF1-6711-C939-2F69070C0F5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="9144000"/>
+          <a:ext cx="8076190" cy="1857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>103848</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>66333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69700425-CE9B-FFBC-BED8-83E0C43F6BB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="11239500"/>
+          <a:ext cx="7419048" cy="2733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>151162</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>113905</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC9856F4-2640-A1E8-90F3-60FA14A8816A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="14668500"/>
+          <a:ext cx="9904762" cy="3161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>27733</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>161524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C340DD5-68DF-0008-1B23-179A100E70BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="18288000"/>
+          <a:ext cx="6733333" cy="3209524"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1522,7 +1807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9C3B07-FCC5-4A8F-ACE3-D8484C9AA250}">
   <dimension ref="A2:B113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
@@ -1562,4 +1847,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3026B40-B613-4CB4-B838-034350EE5C35}">
+  <dimension ref="A2:B96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="S109" sqref="S109"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>